<commit_message>
adjust R script and process for app
</commit_message>
<xml_diff>
--- a/STTR_Caisis_Master Data Dictionary_04042019.xlsx
+++ b/STTR_Caisis_Master Data Dictionary_04042019.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kcolevas/Documents/GitHub/sttr-tgdcc-caisis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apaguiri/Documents/github/DataRepos/sttr-tgdcc-caisis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255A5350-E7A8-AE45-A923-81E5A3C82FC0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D732E6-88D0-E446-9A2B-20B4D7171124}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23400" windowHeight="14500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2316,9 +2316,6 @@
     <t>Date on which Comorbidity diagnosed</t>
   </si>
   <si>
-    <t>Sub-Form</t>
-  </si>
-  <si>
     <t>Review of Symptoms</t>
   </si>
   <si>
@@ -2331,9 +2328,6 @@
     <t>Operating Room Details</t>
   </si>
   <si>
-    <t>Form Notes</t>
-  </si>
-  <si>
     <t>Prostatectomy</t>
   </si>
   <si>
@@ -2734,6 +2728,12 @@
   </si>
   <si>
     <t>Was parathyroid tissue present? Y/N</t>
+  </si>
+  <si>
+    <t>SubForm</t>
+  </si>
+  <si>
+    <t>FormNotes</t>
   </si>
 </sst>
 </file>
@@ -3535,7 +3535,7 @@
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S12" sqref="S12:T12"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3557,10 +3557,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="57" t="s">
-        <v>760</v>
+        <v>898</v>
       </c>
       <c r="C1" s="57" t="s">
-        <v>765</v>
+        <v>899</v>
       </c>
       <c r="D1" s="57" t="s">
         <v>1</v>
@@ -3572,10 +3572,10 @@
         <v>2</v>
       </c>
       <c r="G1" s="57" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="H1" s="57" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="I1" s="58" t="s">
         <v>3</v>
@@ -3584,7 +3584,7 @@
         <v>4</v>
       </c>
       <c r="K1" s="58" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="L1" s="58" t="s">
         <v>5</v>
@@ -3596,7 +3596,7 @@
         <v>6</v>
       </c>
       <c r="O1" s="58" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="P1" s="58" t="s">
         <v>7</v>
@@ -3608,10 +3608,10 @@
         <v>9</v>
       </c>
       <c r="S1" s="58" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="T1" s="58" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -4770,7 +4770,7 @@
         <v>20</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="D33" s="22" t="s">
         <v>230</v>
@@ -4793,7 +4793,7 @@
         <v>20</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="D34" s="22" t="s">
         <v>246</v>
@@ -4819,7 +4819,7 @@
         <v>20</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="D35" s="22" t="s">
         <v>77</v>
@@ -4841,7 +4841,7 @@
         <v>20</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C36" s="23"/>
       <c r="D36" s="23" t="s">
@@ -4864,7 +4864,7 @@
         <v>20</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C37" s="23"/>
       <c r="D37" s="23" t="s">
@@ -4887,7 +4887,7 @@
         <v>20</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C38" s="23"/>
       <c r="D38" s="23" t="s">
@@ -4910,7 +4910,7 @@
         <v>20</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C39" s="23"/>
       <c r="D39" s="23" t="s">
@@ -4933,7 +4933,7 @@
         <v>20</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C40" s="23"/>
       <c r="D40" s="23" t="s">
@@ -4956,7 +4956,7 @@
         <v>20</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C41" s="23"/>
       <c r="D41" s="23" t="s">
@@ -4979,7 +4979,7 @@
         <v>20</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C42" s="23"/>
       <c r="D42" s="23" t="s">
@@ -5002,7 +5002,7 @@
         <v>20</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C43" s="23"/>
       <c r="D43" s="23" t="s">
@@ -5391,7 +5391,7 @@
         <v>34</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C54" s="12"/>
       <c r="D54" s="12" t="s">
@@ -5446,7 +5446,7 @@
         <v>34</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C55" s="12"/>
       <c r="D55" s="12" t="s">
@@ -5499,7 +5499,7 @@
         <v>34</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C56" s="12"/>
       <c r="D56" s="12" t="s">
@@ -5549,7 +5549,7 @@
         <v>34</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C57" s="12"/>
       <c r="D57" s="12" t="s">
@@ -5601,7 +5601,7 @@
         <v>34</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C58" s="12"/>
       <c r="D58" s="28" t="s">
@@ -6210,7 +6210,7 @@
         <v>40</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>168</v>
@@ -6235,7 +6235,7 @@
         <v>40</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>169</v>
@@ -6260,7 +6260,7 @@
         <v>40</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>170</v>
@@ -6285,7 +6285,7 @@
         <v>40</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>171</v>
@@ -6310,7 +6310,7 @@
         <v>40</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>172</v>
@@ -6335,7 +6335,7 @@
         <v>40</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>173</v>
@@ -6360,7 +6360,7 @@
         <v>40</v>
       </c>
       <c r="C79" s="28" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D79" s="28" t="s">
         <v>42</v>
@@ -6385,7 +6385,7 @@
         <v>40</v>
       </c>
       <c r="C80" s="28" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D80" s="28" t="s">
         <v>165</v>
@@ -6410,7 +6410,7 @@
         <v>40</v>
       </c>
       <c r="C81" s="28" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="D81" s="28" t="s">
         <v>248</v>
@@ -6435,7 +6435,7 @@
         <v>40</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="D82" s="28" t="s">
         <v>249</v>
@@ -6460,7 +6460,7 @@
         <v>40</v>
       </c>
       <c r="C83" s="28" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="D83" s="28" t="s">
         <v>250</v>
@@ -6935,13 +6935,13 @@
         <v>40</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D102" s="12" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="E102" s="12" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="F102" s="5" t="s">
         <v>12</v>
@@ -6961,13 +6961,13 @@
         <v>40</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D103" s="12" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="E103" s="12" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="F103" s="5" t="s">
         <v>12</v>
@@ -6987,13 +6987,13 @@
         <v>40</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D104" s="12" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="E104" s="12" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="F104" s="5" t="s">
         <v>12</v>
@@ -7013,13 +7013,13 @@
         <v>40</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D105" s="12" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="E105" s="12" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="F105" s="5" t="s">
         <v>12</v>
@@ -7039,13 +7039,13 @@
         <v>40</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D106" s="12" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="E106" s="12" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="F106" s="5" t="s">
         <v>12</v>
@@ -7065,13 +7065,13 @@
         <v>40</v>
       </c>
       <c r="C107" s="12" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D107" s="12" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="E107" s="12" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="F107" s="5" t="s">
         <v>12</v>
@@ -7091,13 +7091,13 @@
         <v>40</v>
       </c>
       <c r="C108" s="12" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D108" s="12" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="E108" s="12" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="F108" s="5" t="s">
         <v>12</v>
@@ -7117,13 +7117,13 @@
         <v>40</v>
       </c>
       <c r="C109" s="12" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D109" s="12" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="E109" s="12" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="F109" s="5" t="s">
         <v>12</v>
@@ -7143,13 +7143,13 @@
         <v>40</v>
       </c>
       <c r="C110" s="12" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D110" s="12" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="E110" s="12" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="F110" s="5" t="s">
         <v>12</v>
@@ -7166,7 +7166,7 @@
         <v>34</v>
       </c>
       <c r="B111" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C111" s="12"/>
       <c r="D111" s="12" t="s">
@@ -7221,7 +7221,7 @@
         <v>34</v>
       </c>
       <c r="B112" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C112" s="30"/>
       <c r="D112" s="12" t="s">
@@ -7281,7 +7281,7 @@
         <v>34</v>
       </c>
       <c r="B113" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C113" s="10"/>
       <c r="D113" s="12" t="s">
@@ -7341,7 +7341,7 @@
         <v>34</v>
       </c>
       <c r="B114" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C114" s="10"/>
       <c r="D114" s="12" t="s">
@@ -7401,7 +7401,7 @@
         <v>34</v>
       </c>
       <c r="B115" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C115" s="10"/>
       <c r="D115" s="12" t="s">
@@ -7461,7 +7461,7 @@
         <v>34</v>
       </c>
       <c r="B116" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C116" s="10"/>
       <c r="D116" s="12" t="s">
@@ -7515,7 +7515,7 @@
         <v>34</v>
       </c>
       <c r="B117" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C117" s="10"/>
       <c r="D117" s="12" t="s">
@@ -7561,7 +7561,7 @@
         <v>34</v>
       </c>
       <c r="B118" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C118" s="10"/>
       <c r="D118" s="12" t="s">
@@ -7590,7 +7590,7 @@
         <v>34</v>
       </c>
       <c r="B119" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C119" s="10"/>
       <c r="D119" s="12" t="s">
@@ -7650,7 +7650,7 @@
         <v>34</v>
       </c>
       <c r="B120" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C120" s="10"/>
       <c r="D120" s="12" t="s">
@@ -7704,7 +7704,7 @@
         <v>34</v>
       </c>
       <c r="B121" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C121" s="10"/>
       <c r="D121" s="12" t="s">
@@ -7764,7 +7764,7 @@
         <v>34</v>
       </c>
       <c r="B122" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C122" s="10"/>
       <c r="D122" s="12" t="s">
@@ -7824,7 +7824,7 @@
         <v>34</v>
       </c>
       <c r="B123" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C123" s="10"/>
       <c r="D123" s="12" t="s">
@@ -7884,10 +7884,10 @@
         <v>34</v>
       </c>
       <c r="B124" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C124" s="12" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="D124" s="12" t="s">
         <v>32</v>
@@ -7938,10 +7938,10 @@
         <v>34</v>
       </c>
       <c r="B125" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C125" s="12" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="D125" s="12" t="s">
         <v>14</v>
@@ -7989,10 +7989,10 @@
         <v>34</v>
       </c>
       <c r="B126" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C126" s="12" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="D126" s="12" t="s">
         <v>41</v>
@@ -8030,10 +8030,10 @@
         <v>34</v>
       </c>
       <c r="B127" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C127" s="12" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="D127" s="12" t="s">
         <v>70</v>
@@ -8078,10 +8078,10 @@
         <v>34</v>
       </c>
       <c r="B128" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C128" s="12" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="D128" s="12" t="s">
         <v>71</v>
@@ -8129,10 +8129,10 @@
         <v>34</v>
       </c>
       <c r="B129" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C129" s="12" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="D129" s="12" t="s">
         <v>72</v>
@@ -8180,10 +8180,10 @@
         <v>34</v>
       </c>
       <c r="B130" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C130" s="12" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="D130" s="12" t="s">
         <v>73</v>
@@ -8217,10 +8217,10 @@
         <v>34</v>
       </c>
       <c r="B131" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C131" s="12" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D131" s="12" t="s">
         <v>74</v>
@@ -8251,10 +8251,10 @@
         <v>34</v>
       </c>
       <c r="B132" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C132" s="12" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D132" s="12" t="s">
         <v>42</v>
@@ -8286,10 +8286,10 @@
         <v>34</v>
       </c>
       <c r="B133" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C133" s="12" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D133" s="12" t="s">
         <v>41</v>
@@ -8320,10 +8320,10 @@
         <v>34</v>
       </c>
       <c r="B134" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C134" s="12" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D134" s="12" t="s">
         <v>66</v>
@@ -8367,10 +8367,10 @@
         <v>34</v>
       </c>
       <c r="B135" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C135" s="12" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D135" s="12" t="s">
         <v>73</v>
@@ -8408,10 +8408,10 @@
         <v>34</v>
       </c>
       <c r="B136" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C136" s="12" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D136" s="12" t="s">
         <v>24</v>
@@ -8437,10 +8437,10 @@
         <v>34</v>
       </c>
       <c r="B137" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C137" s="12" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D137" s="12" t="s">
         <v>161</v>
@@ -8466,10 +8466,10 @@
         <v>34</v>
       </c>
       <c r="B138" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C138" s="12" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D138" s="12" t="s">
         <v>162</v>
@@ -8495,10 +8495,10 @@
         <v>34</v>
       </c>
       <c r="B139" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C139" s="12" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="D139" s="12" t="s">
         <v>11</v>
@@ -8554,10 +8554,10 @@
         <v>34</v>
       </c>
       <c r="B140" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C140" s="12" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="D140" s="12" t="s">
         <v>75</v>
@@ -8613,10 +8613,10 @@
         <v>34</v>
       </c>
       <c r="B141" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C141" s="12" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="D141" s="12" t="s">
         <v>76</v>
@@ -8672,10 +8672,10 @@
         <v>34</v>
       </c>
       <c r="B142" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C142" s="12" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="D142" s="12" t="s">
         <v>77</v>
@@ -8731,10 +8731,10 @@
         <v>34</v>
       </c>
       <c r="B143" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C143" s="12" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="D143" s="12" t="s">
         <v>367</v>
@@ -8759,10 +8759,10 @@
         <v>34</v>
       </c>
       <c r="B144" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C144" s="12" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="D144" s="12" t="s">
         <v>69</v>
@@ -8818,10 +8818,10 @@
         <v>34</v>
       </c>
       <c r="B145" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C145" s="12" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="D145" s="12" t="s">
         <v>42</v>
@@ -8864,10 +8864,10 @@
         <v>34</v>
       </c>
       <c r="B146" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C146" s="12" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="D146" s="12" t="s">
         <v>41</v>
@@ -8910,10 +8910,10 @@
         <v>34</v>
       </c>
       <c r="B147" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C147" s="12" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="D147" s="12" t="s">
         <v>78</v>
@@ -8956,10 +8956,10 @@
         <v>34</v>
       </c>
       <c r="B148" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C148" s="12" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="D148" s="12" t="s">
         <v>79</v>
@@ -9002,10 +9002,10 @@
         <v>34</v>
       </c>
       <c r="B149" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C149" s="12" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="D149" s="12" t="s">
         <v>80</v>
@@ -9048,10 +9048,10 @@
         <v>34</v>
       </c>
       <c r="B150" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C150" s="12" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="D150" s="12" t="s">
         <v>81</v>
@@ -9094,7 +9094,7 @@
         <v>34</v>
       </c>
       <c r="B151" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C151" s="12" t="s">
         <v>4</v>
@@ -9119,7 +9119,7 @@
         <v>34</v>
       </c>
       <c r="B152" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C152" s="12" t="s">
         <v>4</v>
@@ -9144,7 +9144,7 @@
         <v>34</v>
       </c>
       <c r="B153" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C153" s="12" t="s">
         <v>4</v>
@@ -9169,10 +9169,10 @@
         <v>34</v>
       </c>
       <c r="B154" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C154" s="12" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="D154" s="12" t="s">
         <v>84</v>
@@ -9194,10 +9194,10 @@
         <v>34</v>
       </c>
       <c r="B155" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C155" s="12" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="D155" s="12" t="s">
         <v>85</v>
@@ -9219,10 +9219,10 @@
         <v>34</v>
       </c>
       <c r="B156" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C156" s="12" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="D156" s="12" t="s">
         <v>73</v>
@@ -9244,10 +9244,10 @@
         <v>34</v>
       </c>
       <c r="B157" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C157" s="12" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="D157" s="12" t="s">
         <v>86</v>
@@ -9269,10 +9269,10 @@
         <v>34</v>
       </c>
       <c r="B158" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C158" s="12" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="D158" s="12" t="s">
         <v>87</v>
@@ -9294,10 +9294,10 @@
         <v>34</v>
       </c>
       <c r="B159" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C159" s="12" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="D159" s="12" t="s">
         <v>88</v>
@@ -9319,10 +9319,10 @@
         <v>34</v>
       </c>
       <c r="B160" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C160" s="12" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="D160" s="12" t="s">
         <v>89</v>
@@ -9344,10 +9344,10 @@
         <v>34</v>
       </c>
       <c r="B161" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C161" s="12" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="D161" s="12" t="s">
         <v>90</v>
@@ -9369,10 +9369,10 @@
         <v>34</v>
       </c>
       <c r="B162" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C162" s="12" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="D162" s="12" t="s">
         <v>91</v>
@@ -9394,10 +9394,10 @@
         <v>34</v>
       </c>
       <c r="B163" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C163" s="12" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="D163" s="12" t="s">
         <v>92</v>
@@ -9419,10 +9419,10 @@
         <v>34</v>
       </c>
       <c r="B164" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C164" s="12" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="D164" s="12" t="s">
         <v>93</v>
@@ -9444,10 +9444,10 @@
         <v>34</v>
       </c>
       <c r="B165" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C165" s="12" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="D165" s="12" t="s">
         <v>94</v>
@@ -9469,10 +9469,10 @@
         <v>34</v>
       </c>
       <c r="B166" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C166" s="12" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="D166" s="12" t="s">
         <v>95</v>
@@ -9494,10 +9494,10 @@
         <v>34</v>
       </c>
       <c r="B167" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C167" s="12" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="D167" s="12" t="s">
         <v>96</v>
@@ -9519,10 +9519,10 @@
         <v>34</v>
       </c>
       <c r="B168" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C168" s="12" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="D168" s="12" t="s">
         <v>97</v>
@@ -9544,10 +9544,10 @@
         <v>34</v>
       </c>
       <c r="B169" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C169" s="12" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="D169" s="12" t="s">
         <v>98</v>
@@ -9569,10 +9569,10 @@
         <v>34</v>
       </c>
       <c r="B170" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C170" s="12" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="D170" s="5" t="s">
         <v>99</v>
@@ -9594,10 +9594,10 @@
         <v>34</v>
       </c>
       <c r="B171" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C171" s="31" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="D171" s="31" t="s">
         <v>174</v>
@@ -9619,10 +9619,10 @@
         <v>34</v>
       </c>
       <c r="B172" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C172" s="31" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="D172" s="31" t="s">
         <v>175</v>
@@ -9644,10 +9644,10 @@
         <v>34</v>
       </c>
       <c r="B173" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C173" s="31" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="D173" s="31" t="s">
         <v>176</v>
@@ -9669,10 +9669,10 @@
         <v>34</v>
       </c>
       <c r="B174" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C174" s="31" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="D174" s="31" t="s">
         <v>177</v>
@@ -9694,10 +9694,10 @@
         <v>34</v>
       </c>
       <c r="B175" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C175" s="31" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="D175" s="31" t="s">
         <v>178</v>
@@ -9719,10 +9719,10 @@
         <v>34</v>
       </c>
       <c r="B176" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C176" s="31" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="D176" s="31" t="s">
         <v>179</v>
@@ -9744,10 +9744,10 @@
         <v>34</v>
       </c>
       <c r="B177" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C177" s="31" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="D177" s="31" t="s">
         <v>180</v>
@@ -9769,10 +9769,10 @@
         <v>34</v>
       </c>
       <c r="B178" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C178" s="31" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="D178" s="31" t="s">
         <v>181</v>
@@ -9794,10 +9794,10 @@
         <v>34</v>
       </c>
       <c r="B179" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C179" s="31" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="D179" s="31" t="s">
         <v>182</v>
@@ -9819,10 +9819,10 @@
         <v>34</v>
       </c>
       <c r="B180" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C180" s="31" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="D180" s="31" t="s">
         <v>183</v>
@@ -9844,10 +9844,10 @@
         <v>34</v>
       </c>
       <c r="B181" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C181" s="31" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="D181" s="31" t="s">
         <v>184</v>
@@ -9869,10 +9869,10 @@
         <v>34</v>
       </c>
       <c r="B182" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C182" s="31" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="D182" s="31" t="s">
         <v>88</v>
@@ -9894,10 +9894,10 @@
         <v>34</v>
       </c>
       <c r="B183" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C183" s="31" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="D183" s="31" t="s">
         <v>185</v>
@@ -9919,10 +9919,10 @@
         <v>34</v>
       </c>
       <c r="B184" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C184" s="31" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="D184" s="31" t="s">
         <v>186</v>
@@ -9944,10 +9944,10 @@
         <v>34</v>
       </c>
       <c r="B185" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C185" s="31" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="D185" s="31" t="s">
         <v>187</v>
@@ -9969,10 +9969,10 @@
         <v>34</v>
       </c>
       <c r="B186" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C186" s="31" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="D186" s="31" t="s">
         <v>188</v>
@@ -9994,10 +9994,10 @@
         <v>34</v>
       </c>
       <c r="B187" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C187" s="31" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="D187" s="31" t="s">
         <v>189</v>
@@ -10019,10 +10019,10 @@
         <v>34</v>
       </c>
       <c r="B188" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C188" s="31" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="D188" s="31" t="s">
         <v>190</v>
@@ -10044,10 +10044,10 @@
         <v>34</v>
       </c>
       <c r="B189" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C189" s="31" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="D189" s="31" t="s">
         <v>191</v>
@@ -10069,10 +10069,10 @@
         <v>34</v>
       </c>
       <c r="B190" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C190" s="31" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="D190" s="23" t="s">
         <v>42</v>
@@ -10094,10 +10094,10 @@
         <v>34</v>
       </c>
       <c r="B191" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C191" s="31" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="D191" s="23" t="s">
         <v>165</v>
@@ -10119,10 +10119,10 @@
         <v>34</v>
       </c>
       <c r="B192" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C192" s="31" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="D192" s="23" t="s">
         <v>164</v>
@@ -10144,10 +10144,10 @@
         <v>34</v>
       </c>
       <c r="B193" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C193" s="31" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="D193" s="23" t="s">
         <v>192</v>
@@ -10169,10 +10169,10 @@
         <v>34</v>
       </c>
       <c r="B194" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C194" s="31" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="D194" s="23" t="s">
         <v>193</v>
@@ -10194,10 +10194,10 @@
         <v>34</v>
       </c>
       <c r="B195" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C195" s="31" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="D195" s="23" t="s">
         <v>194</v>
@@ -10219,10 +10219,10 @@
         <v>34</v>
       </c>
       <c r="B196" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C196" s="31" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="D196" s="23" t="s">
         <v>195</v>
@@ -10244,10 +10244,10 @@
         <v>34</v>
       </c>
       <c r="B197" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C197" s="31" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="D197" s="23" t="s">
         <v>196</v>
@@ -10269,10 +10269,10 @@
         <v>34</v>
       </c>
       <c r="B198" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C198" s="31" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="D198" s="23" t="s">
         <v>197</v>
@@ -10294,10 +10294,10 @@
         <v>34</v>
       </c>
       <c r="B199" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C199" s="31" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="D199" s="23" t="s">
         <v>77</v>
@@ -10319,10 +10319,10 @@
         <v>34</v>
       </c>
       <c r="B200" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C200" s="31" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="D200" s="23" t="s">
         <v>198</v>
@@ -10344,10 +10344,10 @@
         <v>34</v>
       </c>
       <c r="B201" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C201" s="31" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="D201" s="23" t="s">
         <v>199</v>
@@ -10369,10 +10369,10 @@
         <v>34</v>
       </c>
       <c r="B202" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C202" s="31" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="D202" s="23" t="s">
         <v>200</v>
@@ -10394,10 +10394,10 @@
         <v>34</v>
       </c>
       <c r="B203" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C203" s="31" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D203" s="31" t="s">
         <v>201</v>
@@ -10419,10 +10419,10 @@
         <v>34</v>
       </c>
       <c r="B204" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C204" s="31" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D204" s="31" t="s">
         <v>178</v>
@@ -10444,10 +10444,10 @@
         <v>34</v>
       </c>
       <c r="B205" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C205" s="31" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D205" s="31" t="s">
         <v>179</v>
@@ -10469,10 +10469,10 @@
         <v>34</v>
       </c>
       <c r="B206" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C206" s="31" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D206" s="31" t="s">
         <v>180</v>
@@ -10494,10 +10494,10 @@
         <v>34</v>
       </c>
       <c r="B207" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C207" s="31" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D207" s="31" t="s">
         <v>202</v>
@@ -10519,10 +10519,10 @@
         <v>34</v>
       </c>
       <c r="B208" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C208" s="31" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D208" s="31" t="s">
         <v>203</v>
@@ -10544,10 +10544,10 @@
         <v>34</v>
       </c>
       <c r="B209" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C209" s="31" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D209" s="31" t="s">
         <v>204</v>
@@ -10569,10 +10569,10 @@
         <v>34</v>
       </c>
       <c r="B210" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C210" s="31" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D210" s="31" t="s">
         <v>205</v>
@@ -10594,10 +10594,10 @@
         <v>34</v>
       </c>
       <c r="B211" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C211" s="31" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D211" s="31" t="s">
         <v>206</v>
@@ -10619,10 +10619,10 @@
         <v>34</v>
       </c>
       <c r="B212" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C212" s="31" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D212" s="31" t="s">
         <v>88</v>
@@ -10644,10 +10644,10 @@
         <v>34</v>
       </c>
       <c r="B213" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C213" s="31" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D213" s="31" t="s">
         <v>207</v>
@@ -10669,10 +10669,10 @@
         <v>34</v>
       </c>
       <c r="B214" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C214" s="31" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D214" s="31" t="s">
         <v>208</v>
@@ -10694,10 +10694,10 @@
         <v>34</v>
       </c>
       <c r="B215" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C215" s="31" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D215" s="31" t="s">
         <v>209</v>
@@ -10719,10 +10719,10 @@
         <v>34</v>
       </c>
       <c r="B216" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C216" s="31" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D216" s="31" t="s">
         <v>86</v>
@@ -10744,10 +10744,10 @@
         <v>34</v>
       </c>
       <c r="B217" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C217" s="31" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D217" s="31" t="s">
         <v>210</v>
@@ -10769,10 +10769,10 @@
         <v>34</v>
       </c>
       <c r="B218" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C218" s="31" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D218" s="31" t="s">
         <v>211</v>
@@ -10794,10 +10794,10 @@
         <v>34</v>
       </c>
       <c r="B219" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C219" s="22" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="D219" s="28" t="s">
         <v>251</v>
@@ -10819,10 +10819,10 @@
         <v>34</v>
       </c>
       <c r="B220" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C220" s="22" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="D220" s="28" t="s">
         <v>252</v>
@@ -10844,10 +10844,10 @@
         <v>34</v>
       </c>
       <c r="B221" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C221" s="22" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="D221" s="28" t="s">
         <v>253</v>
@@ -10869,10 +10869,10 @@
         <v>34</v>
       </c>
       <c r="B222" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C222" s="22" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="D222" s="28" t="s">
         <v>254</v>
@@ -10894,10 +10894,10 @@
         <v>34</v>
       </c>
       <c r="B223" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C223" s="22" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="D223" s="28" t="s">
         <v>255</v>
@@ -10919,10 +10919,10 @@
         <v>34</v>
       </c>
       <c r="B224" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C224" s="22" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="D224" s="28" t="s">
         <v>88</v>
@@ -10944,10 +10944,10 @@
         <v>34</v>
       </c>
       <c r="B225" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C225" s="22" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="D225" s="28" t="s">
         <v>256</v>
@@ -10969,10 +10969,10 @@
         <v>34</v>
       </c>
       <c r="B226" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C226" s="22" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="D226" s="28" t="s">
         <v>257</v>
@@ -10994,10 +10994,10 @@
         <v>34</v>
       </c>
       <c r="B227" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C227" s="22" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="D227" s="28" t="s">
         <v>258</v>
@@ -11019,10 +11019,10 @@
         <v>34</v>
       </c>
       <c r="B228" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C228" s="22" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="D228" s="28" t="s">
         <v>259</v>
@@ -11044,10 +11044,10 @@
         <v>34</v>
       </c>
       <c r="B229" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C229" s="22" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="D229" s="28" t="s">
         <v>260</v>
@@ -11069,10 +11069,10 @@
         <v>34</v>
       </c>
       <c r="B230" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C230" s="22" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="D230" s="28" t="s">
         <v>261</v>
@@ -11094,10 +11094,10 @@
         <v>34</v>
       </c>
       <c r="B231" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C231" s="22" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="D231" s="28" t="s">
         <v>84</v>
@@ -11119,10 +11119,10 @@
         <v>34</v>
       </c>
       <c r="B232" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C232" s="22" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="D232" s="28" t="s">
         <v>262</v>
@@ -11144,10 +11144,10 @@
         <v>34</v>
       </c>
       <c r="B233" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C233" s="22" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="D233" s="28" t="s">
         <v>263</v>
@@ -11169,10 +11169,10 @@
         <v>34</v>
       </c>
       <c r="B234" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C234" s="22" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="D234" s="28" t="s">
         <v>264</v>
@@ -11194,10 +11194,10 @@
         <v>34</v>
       </c>
       <c r="B235" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C235" s="22" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="D235" s="28" t="s">
         <v>265</v>
@@ -11219,7 +11219,7 @@
         <v>34</v>
       </c>
       <c r="B236" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C236" s="6" t="s">
         <v>9</v>
@@ -11244,7 +11244,7 @@
         <v>34</v>
       </c>
       <c r="B237" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C237" s="6" t="s">
         <v>9</v>
@@ -11269,10 +11269,10 @@
         <v>34</v>
       </c>
       <c r="B238" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C238" s="6" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="D238" s="32" t="s">
         <v>311</v>
@@ -11294,10 +11294,10 @@
         <v>34</v>
       </c>
       <c r="B239" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C239" s="6" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="D239" s="32" t="s">
         <v>313</v>
@@ -11319,10 +11319,10 @@
         <v>34</v>
       </c>
       <c r="B240" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C240" s="6" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="D240" s="32" t="s">
         <v>314</v>
@@ -11344,10 +11344,10 @@
         <v>34</v>
       </c>
       <c r="B241" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C241" s="6" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="D241" s="32" t="s">
         <v>315</v>
@@ -11369,10 +11369,10 @@
         <v>34</v>
       </c>
       <c r="B242" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C242" s="6" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="D242" s="32" t="s">
         <v>316</v>
@@ -11394,10 +11394,10 @@
         <v>34</v>
       </c>
       <c r="B243" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C243" s="6" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="D243" s="6" t="s">
         <v>317</v>
@@ -11419,10 +11419,10 @@
         <v>34</v>
       </c>
       <c r="B244" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C244" s="6" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="D244" s="6" t="s">
         <v>315</v>
@@ -11444,10 +11444,10 @@
         <v>34</v>
       </c>
       <c r="B245" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C245" s="6" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="D245" s="6" t="s">
         <v>318</v>
@@ -11469,10 +11469,10 @@
         <v>34</v>
       </c>
       <c r="B246" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C246" s="6" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="D246" s="6" t="s">
         <v>316</v>
@@ -11494,10 +11494,10 @@
         <v>34</v>
       </c>
       <c r="B247" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C247" s="6" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="D247" s="6" t="s">
         <v>319</v>
@@ -11519,10 +11519,10 @@
         <v>34</v>
       </c>
       <c r="B248" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C248" s="6" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="D248" s="6" t="s">
         <v>320</v>
@@ -11544,10 +11544,10 @@
         <v>34</v>
       </c>
       <c r="B249" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C249" s="6" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="D249" s="6" t="s">
         <v>321</v>
@@ -11569,10 +11569,10 @@
         <v>34</v>
       </c>
       <c r="B250" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C250" s="6" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="D250" s="6" t="s">
         <v>322</v>
@@ -11594,7 +11594,7 @@
         <v>34</v>
       </c>
       <c r="B251" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C251" s="33" t="s">
         <v>7</v>
@@ -11619,7 +11619,7 @@
         <v>34</v>
       </c>
       <c r="B252" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C252" s="33" t="s">
         <v>7</v>
@@ -11644,7 +11644,7 @@
         <v>34</v>
       </c>
       <c r="B253" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C253" s="33" t="s">
         <v>7</v>
@@ -11669,7 +11669,7 @@
         <v>34</v>
       </c>
       <c r="B254" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C254" s="33" t="s">
         <v>7</v>
@@ -11694,7 +11694,7 @@
         <v>34</v>
       </c>
       <c r="B255" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C255" s="33" t="s">
         <v>7</v>
@@ -11719,7 +11719,7 @@
         <v>34</v>
       </c>
       <c r="B256" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C256" s="33" t="s">
         <v>7</v>
@@ -11744,10 +11744,10 @@
         <v>34</v>
       </c>
       <c r="B257" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C257" s="33" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="D257" s="28" t="s">
         <v>286</v>
@@ -11769,10 +11769,10 @@
         <v>34</v>
       </c>
       <c r="B258" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C258" s="33" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="D258" s="28" t="s">
         <v>287</v>
@@ -11794,10 +11794,10 @@
         <v>34</v>
       </c>
       <c r="B259" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C259" s="33" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="D259" s="28" t="s">
         <v>288</v>
@@ -11819,10 +11819,10 @@
         <v>34</v>
       </c>
       <c r="B260" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C260" s="33" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="D260" s="28" t="s">
         <v>289</v>
@@ -11844,10 +11844,10 @@
         <v>34</v>
       </c>
       <c r="B261" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C261" s="33" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="D261" s="28" t="s">
         <v>290</v>
@@ -11869,10 +11869,10 @@
         <v>34</v>
       </c>
       <c r="B262" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C262" s="33" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="D262" s="28" t="s">
         <v>291</v>
@@ -11894,10 +11894,10 @@
         <v>34</v>
       </c>
       <c r="B263" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C263" s="33" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="D263" s="28" t="s">
         <v>292</v>
@@ -11919,10 +11919,10 @@
         <v>34</v>
       </c>
       <c r="B264" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C264" s="33" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="D264" s="28" t="s">
         <v>293</v>
@@ -11944,10 +11944,10 @@
         <v>34</v>
       </c>
       <c r="B265" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C265" s="33" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="D265" s="28" t="s">
         <v>294</v>
@@ -11969,10 +11969,10 @@
         <v>34</v>
       </c>
       <c r="B266" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C266" s="33" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="D266" s="28" t="s">
         <v>295</v>
@@ -11994,10 +11994,10 @@
         <v>34</v>
       </c>
       <c r="B267" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C267" s="33" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="D267" s="28" t="s">
         <v>266</v>
@@ -12019,16 +12019,16 @@
         <v>34</v>
       </c>
       <c r="B268" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C268" s="33" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D268" s="28" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="E268" s="28" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="F268" s="34" t="s">
         <v>12</v>
@@ -12045,16 +12045,16 @@
         <v>34</v>
       </c>
       <c r="B269" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C269" s="33" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D269" s="28" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="E269" s="28" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="F269" s="34" t="s">
         <v>12</v>
@@ -12071,16 +12071,16 @@
         <v>34</v>
       </c>
       <c r="B270" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C270" s="33" t="s">
+        <v>815</v>
+      </c>
+      <c r="D270" s="28" t="s">
+        <v>796</v>
+      </c>
+      <c r="E270" s="28" t="s">
         <v>817</v>
-      </c>
-      <c r="D270" s="28" t="s">
-        <v>798</v>
-      </c>
-      <c r="E270" s="28" t="s">
-        <v>819</v>
       </c>
       <c r="F270" s="34" t="s">
         <v>12</v>
@@ -12097,16 +12097,16 @@
         <v>34</v>
       </c>
       <c r="B271" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C271" s="33" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D271" s="28" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="E271" s="28" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="F271" s="34" t="s">
         <v>12</v>
@@ -12123,16 +12123,16 @@
         <v>34</v>
       </c>
       <c r="B272" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C272" s="33" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D272" s="28" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="E272" s="28" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="F272" s="34" t="s">
         <v>12</v>
@@ -12149,16 +12149,16 @@
         <v>34</v>
       </c>
       <c r="B273" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C273" s="33" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D273" s="28" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="E273" s="28" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="F273" s="34" t="s">
         <v>12</v>
@@ -12175,16 +12175,16 @@
         <v>34</v>
       </c>
       <c r="B274" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C274" s="33" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D274" s="28" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="E274" s="28" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="F274" s="34" t="s">
         <v>12</v>
@@ -12201,16 +12201,16 @@
         <v>34</v>
       </c>
       <c r="B275" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C275" s="33" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D275" s="28" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="E275" s="28" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="F275" s="34" t="s">
         <v>12</v>
@@ -12227,16 +12227,16 @@
         <v>34</v>
       </c>
       <c r="B276" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C276" s="33" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D276" s="28" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="E276" s="28" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="F276" s="34" t="s">
         <v>12</v>
@@ -12253,16 +12253,16 @@
         <v>34</v>
       </c>
       <c r="B277" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C277" s="33" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D277" s="28" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="E277" s="28" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="F277" s="34" t="s">
         <v>12</v>
@@ -12279,16 +12279,16 @@
         <v>34</v>
       </c>
       <c r="B278" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C278" s="33" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D278" s="28" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="E278" s="28" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="F278" s="34" t="s">
         <v>12</v>
@@ -12305,16 +12305,16 @@
         <v>34</v>
       </c>
       <c r="B279" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C279" s="33" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D279" s="28" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="E279" s="28" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="F279" s="34" t="s">
         <v>12</v>
@@ -12331,16 +12331,16 @@
         <v>34</v>
       </c>
       <c r="B280" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C280" s="33" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D280" s="28" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="E280" s="28" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="F280" s="34" t="s">
         <v>12</v>
@@ -12357,16 +12357,16 @@
         <v>34</v>
       </c>
       <c r="B281" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C281" s="33" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D281" s="28" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="E281" s="28" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="F281" s="34" t="s">
         <v>12</v>
@@ -12383,16 +12383,16 @@
         <v>34</v>
       </c>
       <c r="B282" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C282" s="33" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D282" s="28" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="E282" s="28" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="F282" s="34" t="s">
         <v>12</v>
@@ -12409,16 +12409,16 @@
         <v>34</v>
       </c>
       <c r="B283" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C283" s="33" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D283" s="28" t="s">
         <v>254</v>
       </c>
       <c r="E283" s="28" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="F283" s="34" t="s">
         <v>12</v>
@@ -12435,16 +12435,16 @@
         <v>34</v>
       </c>
       <c r="B284" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C284" s="33" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D284" s="28" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="E284" s="28" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="F284" s="34" t="s">
         <v>12</v>
@@ -12461,16 +12461,16 @@
         <v>34</v>
       </c>
       <c r="B285" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C285" s="33" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D285" s="28" t="s">
         <v>208</v>
       </c>
       <c r="E285" s="28" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="F285" s="34" t="s">
         <v>12</v>
@@ -12487,16 +12487,16 @@
         <v>34</v>
       </c>
       <c r="B286" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C286" s="33" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D286" s="28" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="E286" s="28" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="F286" s="34" t="s">
         <v>12</v>
@@ -12513,16 +12513,16 @@
         <v>34</v>
       </c>
       <c r="B287" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C287" s="33" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D287" s="28" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="E287" s="28" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="F287" s="34" t="s">
         <v>12</v>
@@ -12539,16 +12539,16 @@
         <v>34</v>
       </c>
       <c r="B288" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C288" s="33" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D288" s="28" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="E288" s="28" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="F288" s="34" t="s">
         <v>12</v>
@@ -12565,16 +12565,16 @@
         <v>34</v>
       </c>
       <c r="B289" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C289" s="33" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="D289" s="28" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="E289" s="28" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="F289" s="34" t="s">
         <v>12</v>
@@ -12591,16 +12591,16 @@
         <v>34</v>
       </c>
       <c r="B290" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C290" s="33" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D290" s="28" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="E290" s="28" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="F290" s="34" t="s">
         <v>12</v>
@@ -12617,16 +12617,16 @@
         <v>34</v>
       </c>
       <c r="B291" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C291" s="33" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D291" s="28" t="s">
         <v>84</v>
       </c>
       <c r="E291" s="28" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="F291" s="34" t="s">
         <v>12</v>
@@ -12643,16 +12643,16 @@
         <v>34</v>
       </c>
       <c r="B292" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C292" s="33" t="s">
+        <v>877</v>
+      </c>
+      <c r="D292" s="28" t="s">
         <v>879</v>
       </c>
-      <c r="D292" s="28" t="s">
-        <v>881</v>
-      </c>
       <c r="E292" s="28" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="F292" s="34" t="s">
         <v>12</v>
@@ -12669,16 +12669,16 @@
         <v>34</v>
       </c>
       <c r="B293" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C293" s="33" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D293" s="28" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="E293" s="28" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="F293" s="34" t="s">
         <v>12</v>
@@ -12695,16 +12695,16 @@
         <v>34</v>
       </c>
       <c r="B294" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C294" s="33" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D294" s="28" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="E294" s="28" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="F294" s="34" t="s">
         <v>12</v>
@@ -12721,16 +12721,16 @@
         <v>34</v>
       </c>
       <c r="B295" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C295" s="33" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D295" s="28" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="E295" s="28" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="F295" s="34" t="s">
         <v>12</v>
@@ -12747,16 +12747,16 @@
         <v>34</v>
       </c>
       <c r="B296" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C296" s="33" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D296" s="28" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="E296" s="28" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="F296" s="34" t="s">
         <v>12</v>
@@ -12773,16 +12773,16 @@
         <v>34</v>
       </c>
       <c r="B297" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C297" s="33" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D297" s="28" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="E297" s="28" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="F297" s="34" t="s">
         <v>12</v>
@@ -12799,16 +12799,16 @@
         <v>34</v>
       </c>
       <c r="B298" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C298" s="33" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D298" s="28" t="s">
         <v>87</v>
       </c>
       <c r="E298" s="28" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="F298" s="34" t="s">
         <v>12</v>
@@ -12825,16 +12825,16 @@
         <v>34</v>
       </c>
       <c r="B299" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C299" s="33" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D299" s="28" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="E299" s="28" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="F299" s="34" t="s">
         <v>12</v>
@@ -12851,16 +12851,16 @@
         <v>34</v>
       </c>
       <c r="B300" s="12" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C300" s="33" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D300" s="28" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="E300" s="28" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="F300" s="34" t="s">
         <v>12</v>
@@ -13310,7 +13310,7 @@
         <v>100</v>
       </c>
       <c r="B316" s="12" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="C316" s="12"/>
       <c r="D316" s="12" t="s">
@@ -13339,7 +13339,7 @@
         <v>100</v>
       </c>
       <c r="B317" s="12" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="C317" s="11"/>
       <c r="D317" s="12" t="s">
@@ -13368,7 +13368,7 @@
         <v>100</v>
       </c>
       <c r="B318" s="12" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="C318" s="11"/>
       <c r="D318" s="12" t="s">
@@ -13394,7 +13394,7 @@
         <v>100</v>
       </c>
       <c r="B319" s="12" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="C319" s="11"/>
       <c r="D319" s="12" t="s">
@@ -13420,7 +13420,7 @@
         <v>100</v>
       </c>
       <c r="B320" s="12" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="C320" s="11"/>
       <c r="D320" s="12" t="s">
@@ -13446,7 +13446,7 @@
         <v>100</v>
       </c>
       <c r="B321" s="12" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="C321" s="6"/>
       <c r="D321" s="6" t="s">
@@ -13475,7 +13475,7 @@
         <v>100</v>
       </c>
       <c r="B322" s="12" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="C322" s="37"/>
       <c r="D322" s="6" t="s">
@@ -13504,7 +13504,7 @@
         <v>100</v>
       </c>
       <c r="B323" s="12" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="C323" s="6"/>
       <c r="D323" s="6" t="s">
@@ -13533,7 +13533,7 @@
         <v>100</v>
       </c>
       <c r="B324" s="12" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="C324" s="6"/>
       <c r="D324" s="6" t="s">
@@ -13557,7 +13557,7 @@
         <v>100</v>
       </c>
       <c r="B325" s="2" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C325" s="2"/>
       <c r="D325" s="3" t="s">
@@ -13580,7 +13580,7 @@
         <v>100</v>
       </c>
       <c r="B326" s="2" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C326" s="2"/>
       <c r="D326" s="3" t="s">
@@ -13603,7 +13603,7 @@
         <v>100</v>
       </c>
       <c r="B327" s="2" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C327" s="2"/>
       <c r="D327" s="3" t="s">
@@ -13626,7 +13626,7 @@
         <v>100</v>
       </c>
       <c r="B328" s="2" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C328" s="2"/>
       <c r="D328" s="3" t="s">
@@ -13649,7 +13649,7 @@
         <v>100</v>
       </c>
       <c r="B329" s="2" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C329" s="2"/>
       <c r="D329" s="3" t="s">
@@ -13672,7 +13672,7 @@
         <v>100</v>
       </c>
       <c r="B330" s="2" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C330" s="2"/>
       <c r="D330" s="3" t="s">
@@ -13695,7 +13695,7 @@
         <v>100</v>
       </c>
       <c r="B331" s="2" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C331" s="2"/>
       <c r="D331" s="3" t="s">
@@ -13718,7 +13718,7 @@
         <v>100</v>
       </c>
       <c r="B332" s="2" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C332" s="2"/>
       <c r="D332" s="3" t="s">
@@ -13741,7 +13741,7 @@
         <v>100</v>
       </c>
       <c r="B333" s="2" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C333" s="2"/>
       <c r="D333" s="3" t="s">
@@ -13764,7 +13764,7 @@
         <v>100</v>
       </c>
       <c r="B334" s="2" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C334" s="2"/>
       <c r="D334" s="3" t="s">
@@ -13787,7 +13787,7 @@
         <v>100</v>
       </c>
       <c r="B335" s="2" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C335" s="2"/>
       <c r="D335" s="3" t="s">
@@ -13810,7 +13810,7 @@
         <v>100</v>
       </c>
       <c r="B336" s="2" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C336" s="2"/>
       <c r="D336" s="3" t="s">
@@ -13833,7 +13833,7 @@
         <v>100</v>
       </c>
       <c r="B337" s="2" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C337" s="2"/>
       <c r="D337" s="3" t="s">
@@ -13856,7 +13856,7 @@
         <v>100</v>
       </c>
       <c r="B338" s="2" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C338" s="2"/>
       <c r="D338" s="3" t="s">
@@ -13879,7 +13879,7 @@
         <v>100</v>
       </c>
       <c r="B339" s="2" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C339" s="2"/>
       <c r="D339" s="3" t="s">
@@ -13902,7 +13902,7 @@
         <v>100</v>
       </c>
       <c r="B340" s="2" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C340" s="29"/>
       <c r="D340" s="3" t="s">
@@ -13925,7 +13925,7 @@
         <v>100</v>
       </c>
       <c r="B341" s="2" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C341" s="29"/>
       <c r="D341" s="3" t="s">
@@ -13948,7 +13948,7 @@
         <v>100</v>
       </c>
       <c r="B342" s="2" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C342" s="29"/>
       <c r="D342" s="3" t="s">
@@ -13971,7 +13971,7 @@
         <v>100</v>
       </c>
       <c r="B343" s="2" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C343" s="29"/>
       <c r="D343" s="3" t="s">
@@ -13994,7 +13994,7 @@
         <v>100</v>
       </c>
       <c r="B344" s="2" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C344" s="29"/>
       <c r="D344" s="3" t="s">
@@ -14017,7 +14017,7 @@
         <v>100</v>
       </c>
       <c r="B345" s="2" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C345" s="29"/>
       <c r="D345" s="3" t="s">
@@ -14040,7 +14040,7 @@
         <v>100</v>
       </c>
       <c r="B346" s="2" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C346" s="29"/>
       <c r="D346" s="3" t="s">
@@ -14063,7 +14063,7 @@
         <v>100</v>
       </c>
       <c r="B347" s="2" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C347" s="29"/>
       <c r="D347" s="3" t="s">
@@ -14086,7 +14086,7 @@
         <v>100</v>
       </c>
       <c r="B348" s="2" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C348" s="29"/>
       <c r="D348" s="3" t="s">
@@ -14109,7 +14109,7 @@
         <v>100</v>
       </c>
       <c r="B349" s="2" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C349" s="29"/>
       <c r="D349" s="3" t="s">
@@ -14132,7 +14132,7 @@
         <v>100</v>
       </c>
       <c r="B350" s="32" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="C350" s="32"/>
       <c r="D350" s="3" t="s">
@@ -14158,7 +14158,7 @@
         <v>100</v>
       </c>
       <c r="B351" s="32" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="C351" s="29"/>
       <c r="D351" s="3" t="s">
@@ -14184,7 +14184,7 @@
         <v>100</v>
       </c>
       <c r="B352" s="32" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="C352" s="29"/>
       <c r="D352" s="3" t="s">
@@ -14210,7 +14210,7 @@
         <v>100</v>
       </c>
       <c r="B353" s="32" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="C353" s="29"/>
       <c r="D353" s="3" t="s">
@@ -14255,7 +14255,7 @@
     </row>
     <row r="355" spans="1:20">
       <c r="A355" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B355" s="13"/>
       <c r="C355" s="13"/>
@@ -14298,7 +14298,7 @@
     </row>
     <row r="356" spans="1:20">
       <c r="A356" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B356" s="13"/>
       <c r="C356" s="13"/>
@@ -14331,7 +14331,7 @@
     </row>
     <row r="357" spans="1:20">
       <c r="A357" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B357" s="13"/>
       <c r="C357" s="13"/>
@@ -14389,7 +14389,7 @@
     </row>
     <row r="358" spans="1:20">
       <c r="A358" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B358" s="13"/>
       <c r="C358" s="13"/>
@@ -14441,7 +14441,7 @@
     </row>
     <row r="359" spans="1:20">
       <c r="A359" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B359" s="13"/>
       <c r="C359" s="13"/>
@@ -14499,7 +14499,7 @@
     </row>
     <row r="360" spans="1:20">
       <c r="A360" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B360" s="13"/>
       <c r="C360" s="13"/>
@@ -14557,7 +14557,7 @@
     </row>
     <row r="361" spans="1:20">
       <c r="A361" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B361" s="13"/>
       <c r="C361" s="13"/>
@@ -14594,7 +14594,7 @@
     </row>
     <row r="362" spans="1:20">
       <c r="A362" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B362" s="13"/>
       <c r="C362" s="13"/>
@@ -14649,7 +14649,7 @@
     </row>
     <row r="363" spans="1:20">
       <c r="A363" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B363" s="13"/>
       <c r="C363" s="13"/>
@@ -14682,7 +14682,7 @@
     </row>
     <row r="364" spans="1:20">
       <c r="A364" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B364" s="13"/>
       <c r="C364" s="13"/>
@@ -14715,7 +14715,7 @@
     </row>
     <row r="365" spans="1:20">
       <c r="A365" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B365" s="13"/>
       <c r="C365" s="13"/>
@@ -14737,7 +14737,7 @@
     </row>
     <row r="366" spans="1:20">
       <c r="A366" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B366" s="13"/>
       <c r="C366" s="13"/>
@@ -14765,7 +14765,7 @@
     </row>
     <row r="367" spans="1:20">
       <c r="A367" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B367" s="13"/>
       <c r="C367" s="13"/>
@@ -14787,7 +14787,7 @@
     </row>
     <row r="368" spans="1:20">
       <c r="A368" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B368" s="13"/>
       <c r="C368" s="13"/>
@@ -14812,7 +14812,7 @@
     </row>
     <row r="369" spans="1:19">
       <c r="A369" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B369" s="13"/>
       <c r="C369" s="13"/>
@@ -14849,7 +14849,7 @@
     </row>
     <row r="370" spans="1:19">
       <c r="A370" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B370" s="13"/>
       <c r="C370" s="13"/>
@@ -14882,7 +14882,7 @@
     </row>
     <row r="371" spans="1:19">
       <c r="A371" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B371" s="13"/>
       <c r="C371" s="13"/>
@@ -14931,7 +14931,7 @@
     </row>
     <row r="372" spans="1:19">
       <c r="A372" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B372" s="13"/>
       <c r="C372" s="13"/>
@@ -14973,7 +14973,7 @@
     </row>
     <row r="373" spans="1:19">
       <c r="A373" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B373" s="6"/>
       <c r="C373" s="6"/>
@@ -14994,7 +14994,7 @@
     </row>
     <row r="374" spans="1:19">
       <c r="A374" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B374" s="6"/>
       <c r="C374" s="6"/>
@@ -15015,7 +15015,7 @@
     </row>
     <row r="375" spans="1:19">
       <c r="A375" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B375" s="6"/>
       <c r="C375" s="6"/>
@@ -15036,7 +15036,7 @@
     </row>
     <row r="376" spans="1:19">
       <c r="A376" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B376" s="6"/>
       <c r="C376" s="6"/>
@@ -15060,10 +15060,10 @@
     </row>
     <row r="377" spans="1:19">
       <c r="A377" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B377" s="12" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C377" s="12"/>
       <c r="D377" s="12" t="s">
@@ -15083,10 +15083,10 @@
     </row>
     <row r="378" spans="1:19">
       <c r="A378" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B378" s="12" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C378" s="10"/>
       <c r="D378" s="12" t="s">
@@ -15106,10 +15106,10 @@
     </row>
     <row r="379" spans="1:19">
       <c r="A379" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B379" s="12" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C379" s="10"/>
       <c r="D379" s="12" t="s">
@@ -15129,10 +15129,10 @@
     </row>
     <row r="380" spans="1:19">
       <c r="A380" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B380" s="12" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C380" s="10"/>
       <c r="D380" s="12" t="s">
@@ -15152,10 +15152,10 @@
     </row>
     <row r="381" spans="1:19">
       <c r="A381" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B381" s="12" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C381" s="10"/>
       <c r="D381" s="12" t="s">
@@ -15175,10 +15175,10 @@
     </row>
     <row r="382" spans="1:19">
       <c r="A382" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B382" s="12" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C382" s="10"/>
       <c r="D382" s="12" t="s">
@@ -15198,10 +15198,10 @@
     </row>
     <row r="383" spans="1:19">
       <c r="A383" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B383" s="12" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C383" s="10"/>
       <c r="D383" s="12" t="s">
@@ -15221,10 +15221,10 @@
     </row>
     <row r="384" spans="1:19">
       <c r="A384" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B384" s="12" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C384" s="10"/>
       <c r="D384" s="12" t="s">
@@ -15244,10 +15244,10 @@
     </row>
     <row r="385" spans="1:20">
       <c r="A385" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B385" s="12" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C385" s="10"/>
       <c r="D385" s="12" t="s">
@@ -15267,10 +15267,10 @@
     </row>
     <row r="386" spans="1:20">
       <c r="A386" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B386" s="12" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C386" s="10"/>
       <c r="D386" s="12" t="s">
@@ -15290,10 +15290,10 @@
     </row>
     <row r="387" spans="1:20">
       <c r="A387" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B387" s="12" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C387" s="10"/>
       <c r="D387" s="12" t="s">
@@ -15313,10 +15313,10 @@
     </row>
     <row r="388" spans="1:20">
       <c r="A388" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B388" s="12" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="C388" s="10"/>
       <c r="D388" s="12" t="s">
@@ -15358,7 +15358,7 @@
     </row>
     <row r="390" spans="1:20">
       <c r="A390" s="21" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B390" s="21"/>
       <c r="C390" s="21"/>
@@ -15416,7 +15416,7 @@
     </row>
     <row r="391" spans="1:20">
       <c r="A391" s="21" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B391" s="10"/>
       <c r="C391" s="10"/>
@@ -15474,7 +15474,7 @@
     </row>
     <row r="392" spans="1:20">
       <c r="A392" s="21" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B392" s="10"/>
       <c r="C392" s="10"/>
@@ -15532,7 +15532,7 @@
     </row>
     <row r="393" spans="1:20">
       <c r="A393" s="21" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B393" s="10"/>
       <c r="C393" s="10"/>
@@ -15587,7 +15587,7 @@
     </row>
     <row r="394" spans="1:20">
       <c r="A394" s="21" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B394" s="10"/>
       <c r="C394" s="10"/>
@@ -15625,7 +15625,7 @@
     </row>
     <row r="395" spans="1:20">
       <c r="A395" s="21" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B395" s="10"/>
       <c r="C395" s="10"/>
@@ -15650,7 +15650,7 @@
     </row>
     <row r="396" spans="1:20">
       <c r="A396" s="21" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B396" s="10"/>
       <c r="C396" s="10"/>
@@ -15703,7 +15703,7 @@
     </row>
     <row r="397" spans="1:20">
       <c r="A397" s="21" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B397" s="10"/>
       <c r="C397" s="10"/>
@@ -15748,7 +15748,7 @@
     </row>
     <row r="398" spans="1:20">
       <c r="A398" s="21" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B398" s="3"/>
       <c r="C398" s="3"/>
@@ -15769,7 +15769,7 @@
     </row>
     <row r="399" spans="1:20">
       <c r="A399" s="21" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B399" s="3"/>
       <c r="C399" s="3"/>
@@ -15790,7 +15790,7 @@
     </row>
     <row r="400" spans="1:20">
       <c r="A400" s="21" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B400" s="3"/>
       <c r="C400" s="3"/>
@@ -15811,7 +15811,7 @@
     </row>
     <row r="401" spans="1:20">
       <c r="A401" s="21" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B401" s="3"/>
       <c r="C401" s="3"/>
@@ -15832,7 +15832,7 @@
     </row>
     <row r="402" spans="1:20">
       <c r="A402" s="21" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B402" s="10"/>
       <c r="C402" s="10"/>
@@ -15884,7 +15884,7 @@
     </row>
     <row r="403" spans="1:20">
       <c r="A403" s="21" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B403" s="10"/>
       <c r="C403" s="10"/>
@@ -15931,7 +15931,7 @@
     </row>
     <row r="404" spans="1:20">
       <c r="A404" s="21" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B404" s="10"/>
       <c r="C404" s="10"/>
@@ -15978,7 +15978,7 @@
     </row>
     <row r="405" spans="1:20">
       <c r="A405" s="21" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B405" s="10"/>
       <c r="C405" s="10"/>
@@ -16025,7 +16025,7 @@
     </row>
     <row r="406" spans="1:20">
       <c r="A406" s="21" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="D406" s="28" t="s">
         <v>275</v>
@@ -16044,7 +16044,7 @@
     </row>
     <row r="407" spans="1:20">
       <c r="A407" s="21" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="D407" s="28" t="s">
         <v>276</v>
@@ -16829,10 +16829,10 @@
       <c r="B436" s="3"/>
       <c r="C436" s="3"/>
       <c r="D436" s="3" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="E436" s="3" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="F436" s="5" t="s">
         <v>12</v>
@@ -16851,10 +16851,10 @@
       <c r="B437" s="3"/>
       <c r="C437" s="3"/>
       <c r="D437" s="3" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="E437" s="3" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="F437" s="5" t="s">
         <v>12</v>
@@ -16873,10 +16873,10 @@
       <c r="B438" s="3"/>
       <c r="C438" s="3"/>
       <c r="D438" s="3" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="E438" s="3" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="F438" s="5" t="s">
         <v>12</v>
@@ -16895,10 +16895,10 @@
       <c r="B439" s="3"/>
       <c r="C439" s="3"/>
       <c r="D439" s="3" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="E439" s="3" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="F439" s="5" t="s">
         <v>12</v>
@@ -16917,10 +16917,10 @@
       <c r="B440" s="3"/>
       <c r="C440" s="3"/>
       <c r="D440" s="3" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="E440" s="3" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="F440" s="5" t="s">
         <v>12</v>
@@ -16939,10 +16939,10 @@
       <c r="B441" s="3"/>
       <c r="C441" s="3"/>
       <c r="D441" s="3" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="E441" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="F441" s="5" t="s">
         <v>12</v>
@@ -16961,10 +16961,10 @@
       <c r="B442" s="3"/>
       <c r="C442" s="3"/>
       <c r="D442" s="3" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="E442" s="3" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="F442" s="5" t="s">
         <v>12</v>
@@ -16983,10 +16983,10 @@
       <c r="B443" s="3"/>
       <c r="C443" s="3"/>
       <c r="D443" s="3" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="E443" s="3" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="F443" s="5" t="s">
         <v>12</v>
@@ -17003,10 +17003,10 @@
       <c r="B444" s="3"/>
       <c r="C444" s="3"/>
       <c r="D444" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="E444" s="3" t="s">
         <v>854</v>
-      </c>
-      <c r="E444" s="3" t="s">
-        <v>856</v>
       </c>
       <c r="F444" s="5" t="s">
         <v>12</v>
@@ -17023,10 +17023,10 @@
       <c r="B445" s="3"/>
       <c r="C445" s="3"/>
       <c r="D445" s="3" t="s">
+        <v>853</v>
+      </c>
+      <c r="E445" s="3" t="s">
         <v>855</v>
-      </c>
-      <c r="E445" s="3" t="s">
-        <v>857</v>
       </c>
       <c r="F445" s="5" t="s">
         <v>12</v>
@@ -18368,7 +18368,7 @@
         <v>137</v>
       </c>
       <c r="B475" s="42" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="C475" s="42"/>
       <c r="D475" s="12" t="s">
@@ -18425,7 +18425,7 @@
         <v>137</v>
       </c>
       <c r="B476" s="42" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="C476" s="1"/>
       <c r="D476" s="12" t="s">
@@ -18559,7 +18559,7 @@
         <v>152</v>
       </c>
       <c r="B479" s="5" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="C479" s="5"/>
       <c r="D479" s="5" t="s">
@@ -18616,7 +18616,7 @@
         <v>152</v>
       </c>
       <c r="B480" s="5" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="C480" s="44"/>
       <c r="D480" s="5" t="s">
@@ -18673,7 +18673,7 @@
         <v>152</v>
       </c>
       <c r="B481" s="5" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="C481" s="45"/>
       <c r="D481" s="5" t="s">
@@ -19023,7 +19023,7 @@
         <v>233</v>
       </c>
       <c r="B495" s="12" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C495" s="12"/>
       <c r="D495" s="12" t="s">
@@ -19058,7 +19058,7 @@
         <v>233</v>
       </c>
       <c r="B496" s="12" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C496" s="10"/>
       <c r="D496" s="12" t="s">
@@ -19093,7 +19093,7 @@
         <v>233</v>
       </c>
       <c r="B497" s="12" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C497" s="10"/>
       <c r="D497" s="12" t="s">
@@ -19122,14 +19122,14 @@
         <v>233</v>
       </c>
       <c r="B498" s="12" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C498" s="10"/>
       <c r="D498" s="12" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="E498" s="12" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="F498" s="5" t="s">
         <v>12</v>
@@ -19738,7 +19738,7 @@
         <v>147</v>
       </c>
       <c r="B515" s="3" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="C515" s="3"/>
       <c r="D515" s="3" t="s">
@@ -19794,7 +19794,7 @@
         <v>147</v>
       </c>
       <c r="B516" s="3" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="C516" s="52"/>
       <c r="D516" s="3" t="s">
@@ -19850,7 +19850,7 @@
         <v>147</v>
       </c>
       <c r="B517" s="3" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="C517" s="52"/>
       <c r="D517" s="3" t="s">
@@ -19906,7 +19906,7 @@
         <v>147</v>
       </c>
       <c r="B518" s="3" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="C518" s="52"/>
       <c r="D518" s="3" t="s">
@@ -19962,7 +19962,7 @@
         <v>147</v>
       </c>
       <c r="B519" s="3" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="C519" s="52"/>
       <c r="D519" s="3" t="s">
@@ -20018,7 +20018,7 @@
         <v>147</v>
       </c>
       <c r="B520" s="3" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="C520" s="52"/>
       <c r="D520" s="3" t="s">
@@ -20074,7 +20074,7 @@
         <v>147</v>
       </c>
       <c r="B521" s="3" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="C521" s="52"/>
       <c r="D521" s="3" t="s">

</xml_diff>